<commit_message>
Bergey model completed. Ready for QED adaption.
</commit_message>
<xml_diff>
--- a/Bergey-Excel-15/WS_VDC.xlsx
+++ b/Bergey-Excel-15/WS_VDC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Bergy\Bergy Final Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Flatirons Campus Row 1 Wind Turbines\Bergey-Excel-15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A822B3E0-F40A-44B2-BD2B-63D7C4FD2E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0381F6F4-D6F6-42C1-B7C8-0B692AAE61E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="1305" windowWidth="9810" windowHeight="10800" xr2:uid="{8CBE82B4-4A62-44DC-B4EE-110EBD052003}"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="5475" windowHeight="10305" xr2:uid="{8CBE82B4-4A62-44DC-B4EE-110EBD052003}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
         <v>80</v>
       </c>
       <c r="C2">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="D2" s="1">
         <v>1125.6150305988692</v>
@@ -470,7 +470,7 @@
         <v>100</v>
       </c>
       <c r="C3">
-        <v>450</v>
+        <v>422</v>
       </c>
       <c r="D3" s="1">
         <v>2198.4668566384162</v>
@@ -484,10 +484,10 @@
         <v>120</v>
       </c>
       <c r="C4">
-        <v>555</v>
+        <v>520</v>
       </c>
       <c r="D4" s="1">
-        <v>3798.9507282711834</v>
+        <v>3798.9507282711802</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -498,7 +498,7 @@
         <v>130</v>
       </c>
       <c r="C5">
-        <v>615</v>
+        <v>558</v>
       </c>
       <c r="D5" s="1">
         <v>6005.8852479052694</v>
@@ -512,7 +512,7 @@
         <v>135</v>
       </c>
       <c r="C6">
-        <v>640</v>
+        <v>560</v>
       </c>
       <c r="D6" s="3">
         <v>8746.2114051619374</v>
@@ -526,7 +526,7 @@
         <v>135</v>
       </c>
       <c r="C7">
-        <v>635</v>
+        <v>533</v>
       </c>
       <c r="D7" s="3">
         <v>11263.331818948067</v>
@@ -540,7 +540,7 @@
         <v>135</v>
       </c>
       <c r="C8">
-        <v>630</v>
+        <v>510</v>
       </c>
       <c r="D8" s="3">
         <v>13381.009695151406</v>
@@ -554,7 +554,7 @@
         <v>135</v>
       </c>
       <c r="C9">
-        <v>625</v>
+        <v>490</v>
       </c>
       <c r="D9" s="3">
         <v>15074.716023946317</v>
@@ -568,7 +568,7 @@
         <v>135</v>
       </c>
       <c r="C10">
-        <v>625</v>
+        <v>475</v>
       </c>
       <c r="D10" s="3">
         <v>16364.468896464674</v>
@@ -582,7 +582,7 @@
         <v>135</v>
       </c>
       <c r="C11">
-        <v>620</v>
+        <v>458</v>
       </c>
       <c r="D11" s="3">
         <v>17881.848410832125</v>
@@ -596,7 +596,7 @@
         <v>135</v>
       </c>
       <c r="C12">
-        <v>620</v>
+        <v>453</v>
       </c>
       <c r="D12" s="3">
         <v>18252.17002603547</v>
@@ -610,7 +610,7 @@
         <v>135</v>
       </c>
       <c r="C13">
-        <v>620</v>
+        <v>459</v>
       </c>
       <c r="D13" s="3">
         <v>17771.749819195316</v>
@@ -624,7 +624,7 @@
         <v>135</v>
       </c>
       <c r="C14">
-        <v>625</v>
+        <v>480</v>
       </c>
       <c r="D14" s="3">
         <v>16004.942021430328</v>
@@ -638,7 +638,7 @@
         <v>135</v>
       </c>
       <c r="C15">
-        <v>630</v>
+        <v>507</v>
       </c>
       <c r="D15" s="3">
         <v>13615.97113089877</v>
@@ -652,7 +652,7 @@
         <v>135</v>
       </c>
       <c r="C16">
-        <v>635</v>
+        <v>533</v>
       </c>
       <c r="D16" s="3">
         <v>11217.180768065075</v>
@@ -666,7 +666,7 @@
         <v>135</v>
       </c>
       <c r="C17">
-        <v>635</v>
+        <v>554</v>
       </c>
       <c r="D17" s="3">
         <v>9351.1945743411834</v>
@@ -680,7 +680,7 @@
         <v>135</v>
       </c>
       <c r="C18">
-        <v>640</v>
+        <v>563</v>
       </c>
       <c r="D18" s="3">
         <v>8517.1753324812853</v>

</xml_diff>